<commit_message>
Test copy data from manmos to excel
</commit_message>
<xml_diff>
--- a/Document/masterConfig.xlsx
+++ b/Document/masterConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="3720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="3720" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Robot" sheetId="8" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="169">
   <si>
     <t>name</t>
   </si>
@@ -641,6 +641,39 @@
   </si>
   <si>
     <t>tempPath</t>
+  </si>
+  <si>
+    <t>collectionDataError</t>
+  </si>
+  <si>
+    <t>{
+"sendTo":"{sendTo}",
+"subject":"{robotName} - Failed to load collection data window.",
+"body":
+"&lt;html&gt;
+&lt;head&gt;
+&lt;style&gt;
+div {font-family:Cordia New, Arial, sans-serif; font-size:24px;}
+&lt;/style&gt;
+&lt;/head&gt;
+&lt;body&gt;
+&lt;div&gt;
+Dear all,&lt;br/&gt;&lt;br/&gt;
+Robot couldn't load collection data from manmos.&lt;br/&gt;
+Because manmos working slowly more than 5 minute&lt;br/&gt;&lt;br/&gt;
+Thank you&lt;br/&gt;&lt;br/&gt;
+&lt;/div&gt;
+&lt;div&gt;
+&lt;b&gt;Robotic Process Automation (RPA)&lt;br/&gt;
+APP Department - Head Office&lt;br/&gt;
+&lt;img src='https://www.jobtni.com/files/company/logo/281.jpg' alt='' height='80'&gt;&lt;br/&gt;
+NHK Spring (Thailand) CO.,LTD.&lt;br/&gt;
+Phone : (+66)2-730-2200 Ext: 2433&lt;br/&gt;
+E-mail : &lt;/b&gt;&lt;a href='mailto:chakrit.pok@nhkspg.co.th?Subject=Contact Problem' target='_top'&gt;chakrit.pok@nhkspg.co.th&lt;/a&gt;
+&lt;/div&gt;
+&lt;/body&gt;
+&lt;/html&gt;"
+}</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1858,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1910,9 +1943,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
+    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>168</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Complete write as csv
</commit_message>
<xml_diff>
--- a/Document/masterConfig.xlsx
+++ b/Document/masterConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="3720" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="3720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Robot" sheetId="8" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="333">
   <si>
     <t>name</t>
   </si>
@@ -53,24 +53,6 @@
     <t>teratermPath</t>
   </si>
   <si>
-    <t>backupPath</t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
-    <t>masterPath</t>
-  </si>
-  <si>
-    <t>D:\Robot-for-test\RFID\input</t>
-  </si>
-  <si>
-    <t>D:\Robot-for-test\RFID\backup</t>
-  </si>
-  <si>
-    <t>D:\Robot-for-test\RFID\master</t>
-  </si>
-  <si>
     <t>chakrit.pok@nhkspg.co.th;</t>
   </si>
   <si>
@@ -83,45 +65,7 @@
     <t>/home/</t>
   </si>
   <si>
-    <t>outputPath</t>
-  </si>
-  <si>
-    <t>D:\Robot-for-test\RFID\output</t>
-  </si>
-  <si>
     <t>inputPath</t>
-  </si>
-  <si>
-    <t>{
-"sendTo":"{sendTo}",
-"subject":"{robotName} - Failed PO Receipt From RFID file {fileName}.",
-"body":
-"&lt;html&gt;
-&lt;head&gt;
-&lt;style&gt;
-div {font-family:Cordia New, Arial, sans-serif; font-size:24px;}
-&lt;/style&gt;
-&lt;/head&gt;
-&lt;body&gt;
-&lt;div&gt;
-Dear all,&lt;br/&gt;&lt;br/&gt;
-Please kindly be informed that RFID file &lt;span style='color:blue'&gt;{fileName}&lt;/span&gt;.&lt;br/&gt;
-have been updated &lt;font color='red'&gt;failed!!&lt;/font&gt; for today.&lt;/br&gt;
-Because Kanban barcode is inused or incorrect&lt;br/&gt;
-Please check status in the receipt file from attached file.&lt;br/&gt;&lt;br/&gt;
-Thank you&lt;br/&gt;&lt;br/&gt;
-&lt;/div&gt;
-&lt;div&gt;
-&lt;b&gt;Robotic Process Automation (RPA)&lt;br/&gt;
-APP Department - Head Office&lt;br/&gt;
-&lt;img src='https://www.jobtni.com/files/company/logo/281.jpg' alt='' height='80'&gt;&lt;br/&gt;
-NHK Spring (Thailand) CO.,LTD.&lt;br/&gt;
-Phone : (+66)2-730-2200 Ext: 2433&lt;br/&gt;
-E-mail : &lt;/b&gt;&lt;a href='mailto:chakrit.pok@nhkspg.co.th?Subject=Contact Problem' target='_top'&gt;chakrit.pok@nhkspg.co.th&lt;/a&gt;
-&lt;/div&gt;
-&lt;/body&gt;
-&lt;/html&gt;"
-}</t>
   </si>
   <si>
     <t>{
@@ -192,9 +136,6 @@
   </si>
   <si>
     <t>for determine start position in report excel</t>
-  </si>
-  <si>
-    <t>D:\Robot-for-test\RFID\templete</t>
   </si>
   <si>
     <t>Lot info template.xlsx</t>
@@ -343,30 +284,15 @@
     <t>W</t>
   </si>
   <si>
-    <t>SI_BP</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>SI_LB</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>SI_FX</t>
-  </si>
-  <si>
-    <t>SI_PZT1</t>
-  </si>
-  <si>
     <t>AB</t>
   </si>
   <si>
-    <t>SI_PZT2</t>
-  </si>
-  <si>
     <t>AC</t>
   </si>
   <si>
@@ -415,33 +341,6 @@
     <t>for determine column Tray Initial in wip excel</t>
   </si>
   <si>
-    <t>tempColOqaLot</t>
-  </si>
-  <si>
-    <t>OQA Lot</t>
-  </si>
-  <si>
-    <t>tempColProdLot</t>
-  </si>
-  <si>
-    <t>Production Lot</t>
-  </si>
-  <si>
-    <t>tempColW</t>
-  </si>
-  <si>
-    <t>tempColX</t>
-  </si>
-  <si>
-    <t>tempColY</t>
-  </si>
-  <si>
-    <t>tempColAB</t>
-  </si>
-  <si>
-    <t>tempColAC</t>
-  </si>
-  <si>
     <t>for determine column OQA Lot  in report excel</t>
   </si>
   <si>
@@ -463,21 +362,9 @@
     <t>for determine column SI_PZT2 in report excel</t>
   </si>
   <si>
-    <t>tempColTray</t>
-  </si>
-  <si>
-    <t>Tray 1D Barcode</t>
-  </si>
-  <si>
     <t>for determine column Tray 1D Barcode in report excel</t>
   </si>
   <si>
-    <t>tempColPackDate</t>
-  </si>
-  <si>
-    <t>Packing date</t>
-  </si>
-  <si>
     <t>for determine column Packing date in report excel</t>
   </si>
   <si>
@@ -508,24 +395,6 @@
     <t>mainPath</t>
   </si>
   <si>
-    <t>D:\Robot-for-test\RFID</t>
-  </si>
-  <si>
-    <t>locatColServer</t>
-  </si>
-  <si>
-    <t>locatColDomain</t>
-  </si>
-  <si>
-    <t>locatColType</t>
-  </si>
-  <si>
-    <t>locatColReg</t>
-  </si>
-  <si>
-    <t>locatColProcess</t>
-  </si>
-  <si>
     <t>Data Type</t>
   </si>
   <si>
@@ -541,69 +410,12 @@
     <t>Process name (Sheet name)</t>
   </si>
   <si>
-    <t>locatPosition</t>
-  </si>
-  <si>
     <t>B4</t>
   </si>
   <si>
-    <t>tempPosition</t>
-  </si>
-  <si>
-    <t>tempSheet</t>
-  </si>
-  <si>
-    <t>custSheet</t>
-  </si>
-  <si>
-    <t>contSheet</t>
-  </si>
-  <si>
-    <t>custPosition</t>
-  </si>
-  <si>
-    <t>custColLot</t>
-  </si>
-  <si>
-    <t>custColModel</t>
-  </si>
-  <si>
-    <t>custColRemark</t>
-  </si>
-  <si>
-    <t>custValRemark</t>
-  </si>
-  <si>
-    <t>contColPartNum</t>
-  </si>
-  <si>
-    <t>contPosition</t>
-  </si>
-  <si>
-    <t>contColDigit</t>
-  </si>
-  <si>
-    <t>contColModel</t>
-  </si>
-  <si>
-    <t>contColFileName</t>
-  </si>
-  <si>
-    <t>contName</t>
-  </si>
-  <si>
-    <t>tempName</t>
-  </si>
-  <si>
-    <t>locatSheet</t>
-  </si>
-  <si>
     <t>Manmos Location</t>
   </si>
   <si>
-    <t>locatValTypeIqa</t>
-  </si>
-  <si>
     <t>IQA data</t>
   </si>
   <si>
@@ -631,16 +443,7 @@
     <t>Inprocess</t>
   </si>
   <si>
-    <t>locatValTypeInp</t>
-  </si>
-  <si>
     <t>OQA</t>
-  </si>
-  <si>
-    <t>locatValTypeOqa</t>
-  </si>
-  <si>
-    <t>tempPath</t>
   </si>
   <si>
     <t>collectionDataError</t>
@@ -674,6 +477,692 @@
 &lt;/body&gt;
 &lt;/html&gt;"
 }</t>
+  </si>
+  <si>
+    <t>tempManmos</t>
+  </si>
+  <si>
+    <t>temp.xlsx</t>
+  </si>
+  <si>
+    <t>Inprocess Lot sampling</t>
+  </si>
+  <si>
+    <t>for determine column Inprocess Lot sampling in location excel</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>for determine column Status in location excel</t>
+  </si>
+  <si>
+    <t>regLotNotFound</t>
+  </si>
+  <si>
+    <t>Input Lot</t>
+  </si>
+  <si>
+    <t>for determine column Input Lot in location excel</t>
+  </si>
+  <si>
+    <t>lotInfoName</t>
+  </si>
+  <si>
+    <t>for determine start position in Lot Info excel</t>
+  </si>
+  <si>
+    <t>Data sample / lot</t>
+  </si>
+  <si>
+    <t>for determine column Data sample / lot in location excel</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Column0</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>wipColItemNumber</t>
+  </si>
+  <si>
+    <t>Item Number</t>
+  </si>
+  <si>
+    <t>for determine column Item Number in wip excel</t>
+  </si>
+  <si>
+    <t>Production Lot</t>
+  </si>
+  <si>
+    <t>colProdLot</t>
+  </si>
+  <si>
+    <t>OQA Lot</t>
+  </si>
+  <si>
+    <t>colOqaLot</t>
+  </si>
+  <si>
+    <t>{
+"sendTo":"{sendTo}",
+"subject":"{robotName} - ผลการค้นหาไม่สำเร็จ",
+"body":
+"&lt;html&gt;
+&lt;head&gt;
+&lt;style&gt;
+div {font-family:Cordia New, Arial, sans-serif; font-size:24px;}
+&lt;/style&gt;
+&lt;/head&gt;
+&lt;body&gt;
+&lt;div&gt;
+เรียนผู้เกี่ยวข้อง,&lt;br/&gt;&lt;br/&gt;
+{ul}&lt;br/&gt;
+ขอบคุณครับ&lt;br/&gt;&lt;br/&gt;
+&lt;/div&gt;
+&lt;div&gt;
+&lt;b&gt;Robotic Process Automation (RPA)&lt;br/&gt;
+APP Department - Head Office&lt;br/&gt;
+&lt;img src='https://www.jobtni.com/files/company/logo/281.jpg' alt='' height='80'&gt;&lt;br/&gt;
+NHK Spring (Thailand) CO.,LTD.&lt;br/&gt;
+Phone : (+66)2-730-2200 Ext: 2433&lt;br/&gt;
+E-mail : &lt;/b&gt;&lt;a href='mailto:chakrit.pok@nhkspg.co.th?Subject=Contact Problem' target='_top'&gt;chakrit.pok@nhkspg.co.th&lt;/a&gt;
+&lt;/div&gt;
+&lt;/body&gt;
+&lt;/html&gt;"
+}</t>
+  </si>
+  <si>
+    <t>S:\EDP\RPA\RPA Phase7\DDS\Industry4.0\Example Rev.03\00.Input</t>
+  </si>
+  <si>
+    <t>S:\EDP\RPA\RPA Phase7\DDS\Industry4.0\Example Rev.03\01.Raw data Manmos\Master</t>
+  </si>
+  <si>
+    <t>S:\EDP\RPA\RPA Phase7\DDS\Industry4.0\Example Rev.03\02.Master output\Master</t>
+  </si>
+  <si>
+    <t>S:\EDP\RPA\RPA Phase7\DDS\Industry4.0\Example Rev.03\02.Master output</t>
+  </si>
+  <si>
+    <t>resultPath</t>
+  </si>
+  <si>
+    <t>controlPath</t>
+  </si>
+  <si>
+    <t>lotInfoMasterPath</t>
+  </si>
+  <si>
+    <t>lotInfoPath</t>
+  </si>
+  <si>
+    <t>S:\EDP\RPA\RPA Phase7\DDS\Industry4.0\Example Rev.03\01.Raw data Manmos\Lot infor form MFG-PRO</t>
+  </si>
+  <si>
+    <t>rawMasterPath</t>
+  </si>
+  <si>
+    <t>rawPath</t>
+  </si>
+  <si>
+    <t>S:\EDP\RPA\RPA Phase7\DDS\Industry4.0\Example Rev.03\01.Raw data Manmos</t>
+  </si>
+  <si>
+    <t>controlName</t>
+  </si>
+  <si>
+    <t>lotInfoSheet</t>
+  </si>
+  <si>
+    <t>lotInfoColOqaLot</t>
+  </si>
+  <si>
+    <t>lotInfoColProdLot</t>
+  </si>
+  <si>
+    <t>lotInfoColW</t>
+  </si>
+  <si>
+    <t>lotInfoColX</t>
+  </si>
+  <si>
+    <t>lotInfoColY</t>
+  </si>
+  <si>
+    <t>lotInfoColAB</t>
+  </si>
+  <si>
+    <t>lotInfoColAC</t>
+  </si>
+  <si>
+    <t>lotInfoColTray</t>
+  </si>
+  <si>
+    <t>lotInfoColPackDate</t>
+  </si>
+  <si>
+    <t>lotInfoPositionW</t>
+  </si>
+  <si>
+    <t>lotInfoPositionR</t>
+  </si>
+  <si>
+    <t>rawSheet</t>
+  </si>
+  <si>
+    <t>rawPosition</t>
+  </si>
+  <si>
+    <t>rawColType</t>
+  </si>
+  <si>
+    <t>rawColDomain</t>
+  </si>
+  <si>
+    <t>rawColServer</t>
+  </si>
+  <si>
+    <t>rawColReg</t>
+  </si>
+  <si>
+    <t>rawColProcess</t>
+  </si>
+  <si>
+    <t>rawColSample</t>
+  </si>
+  <si>
+    <t>rawColLot</t>
+  </si>
+  <si>
+    <t>rawColInputLot</t>
+  </si>
+  <si>
+    <t>rawColStatus</t>
+  </si>
+  <si>
+    <t>rawValTypeIqa</t>
+  </si>
+  <si>
+    <t>rawValTypeInp</t>
+  </si>
+  <si>
+    <t>rawValTypeOqa</t>
+  </si>
+  <si>
+    <t>controlSheet</t>
+  </si>
+  <si>
+    <t>inputSheet</t>
+  </si>
+  <si>
+    <t>inputPosition</t>
+  </si>
+  <si>
+    <t>inputColLot</t>
+  </si>
+  <si>
+    <t>inputColModel</t>
+  </si>
+  <si>
+    <t>inputColRemark</t>
+  </si>
+  <si>
+    <t>inputValRemark</t>
+  </si>
+  <si>
+    <t>controlPosition</t>
+  </si>
+  <si>
+    <t>controlColDigit</t>
+  </si>
+  <si>
+    <t>controlColModel</t>
+  </si>
+  <si>
+    <t>controlColPartNum</t>
+  </si>
+  <si>
+    <t>controlColFileName</t>
+  </si>
+  <si>
+    <t>S:\EDP\RPA\RPA Phase7\DDS\Industry4.0\Example Rev.03\</t>
+  </si>
+  <si>
+    <t>outputName</t>
+  </si>
+  <si>
+    <t>Pine2.2.2 Master output{lot}.xlsx</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Back up</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>for determine start position control row in output master excel</t>
+  </si>
+  <si>
+    <t>for determine start position control column in output master excel</t>
+  </si>
+  <si>
+    <t>Data sampling</t>
+  </si>
+  <si>
+    <t>Sheet name</t>
+  </si>
+  <si>
+    <t>for determine column Production Lot for control row in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column Data sampling for control row in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column Column input data for control column in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column Column input MEA Date for control column in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column Sheet name for control row in output master excel</t>
+  </si>
+  <si>
+    <t>for determine start position template in output master excel</t>
+  </si>
+  <si>
+    <t>B3:D13</t>
+  </si>
+  <si>
+    <t>controlColTab</t>
+  </si>
+  <si>
+    <t>controlColEC</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>EC no.</t>
+  </si>
+  <si>
+    <t>for determine columnTab in control excel</t>
+  </si>
+  <si>
+    <t>for determine column EC no. in control excel</t>
+  </si>
+  <si>
+    <t>SI_BP</t>
+  </si>
+  <si>
+    <t>SI_LB</t>
+  </si>
+  <si>
+    <t>SI_FX</t>
+  </si>
+  <si>
+    <t>SI_PZT1</t>
+  </si>
+  <si>
+    <t>SI_PZT2</t>
+  </si>
+  <si>
+    <t>Tray 1D Barcode</t>
+  </si>
+  <si>
+    <t>Packing date</t>
+  </si>
+  <si>
+    <t>colBP</t>
+  </si>
+  <si>
+    <t>colLB</t>
+  </si>
+  <si>
+    <t>colFX</t>
+  </si>
+  <si>
+    <t>colPZT1</t>
+  </si>
+  <si>
+    <t>colPZT2</t>
+  </si>
+  <si>
+    <t>colTray</t>
+  </si>
+  <si>
+    <t>colPackDate</t>
+  </si>
+  <si>
+    <t>NCA1</t>
+  </si>
+  <si>
+    <t>NCA2</t>
+  </si>
+  <si>
+    <t>NCA3</t>
+  </si>
+  <si>
+    <t>NCA4</t>
+  </si>
+  <si>
+    <t>NCA5</t>
+  </si>
+  <si>
+    <t>CA1</t>
+  </si>
+  <si>
+    <t>CA2</t>
+  </si>
+  <si>
+    <t>CA3</t>
+  </si>
+  <si>
+    <t>CA4</t>
+  </si>
+  <si>
+    <t>CA5</t>
+  </si>
+  <si>
+    <t>PZT1</t>
+  </si>
+  <si>
+    <t>PZT2</t>
+  </si>
+  <si>
+    <t>PZT3</t>
+  </si>
+  <si>
+    <t>PZT4</t>
+  </si>
+  <si>
+    <t>Damper</t>
+  </si>
+  <si>
+    <t>Flexure</t>
+  </si>
+  <si>
+    <t>LoadBeam</t>
+  </si>
+  <si>
+    <t>BasePlate</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>EC_No.</t>
+  </si>
+  <si>
+    <t>LOT</t>
+  </si>
+  <si>
+    <t>SUB_LOT</t>
+  </si>
+  <si>
+    <t>LOT_SEQ_No.</t>
+  </si>
+  <si>
+    <t>SUB_LOT_SEQ_No.</t>
+  </si>
+  <si>
+    <t>for determine column Part Number in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column EC_No. in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column Tab in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column LOT in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column SUB_LOT in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column LOT_SEQ_No. in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column SUB_LOT_SEQ_No. in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column Flexure in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column LoadBeam in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column BasePlate in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column PZT1 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column PZT2 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column PZT3 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column PZT4 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column Damper in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column CA1 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column CA2 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column CA3 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column CA4 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column CA5 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column NCA1 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column NCA2 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column NCA3 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column NCA4 in output master excel</t>
+  </si>
+  <si>
+    <t>for determine column NCA5 in output master excel</t>
+  </si>
+  <si>
+    <t>col_PartNum</t>
+  </si>
+  <si>
+    <t>col_EC</t>
+  </si>
+  <si>
+    <t>col_Tab</t>
+  </si>
+  <si>
+    <t>col_Lot</t>
+  </si>
+  <si>
+    <t>col_SubLot</t>
+  </si>
+  <si>
+    <t>col_LotSeq</t>
+  </si>
+  <si>
+    <t>col_SubLotSeq</t>
+  </si>
+  <si>
+    <t>col_FX</t>
+  </si>
+  <si>
+    <t>col_LB</t>
+  </si>
+  <si>
+    <t>col_BP</t>
+  </si>
+  <si>
+    <t>col_PZT1</t>
+  </si>
+  <si>
+    <t>col_PZT2</t>
+  </si>
+  <si>
+    <t>col_PZT3</t>
+  </si>
+  <si>
+    <t>col_PZT4</t>
+  </si>
+  <si>
+    <t>col_Damper</t>
+  </si>
+  <si>
+    <t>col_CA1</t>
+  </si>
+  <si>
+    <t>col_CA2</t>
+  </si>
+  <si>
+    <t>col_CA3</t>
+  </si>
+  <si>
+    <t>col_CA4</t>
+  </si>
+  <si>
+    <t>col_CA5</t>
+  </si>
+  <si>
+    <t>col_NCA1</t>
+  </si>
+  <si>
+    <t>col_NCA2</t>
+  </si>
+  <si>
+    <t>col_NCA3</t>
+  </si>
+  <si>
+    <t>col_NCA4</t>
+  </si>
+  <si>
+    <t>col_NCA5</t>
+  </si>
+  <si>
+    <t>rawValPosition</t>
+  </si>
+  <si>
+    <t>for determine start value position in location excel</t>
+  </si>
+  <si>
+    <t>Row number (Position)</t>
+  </si>
+  <si>
+    <t>for determine column Row number (Position) in output master excel</t>
+  </si>
+  <si>
+    <t>Column name start input data</t>
+  </si>
+  <si>
+    <t>Column name input MEA Date</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>col_ValuePosition</t>
+  </si>
+  <si>
+    <t>for determine start position value in output master excel</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>comRowPosition</t>
+  </si>
+  <si>
+    <t>comColumnPosition</t>
+  </si>
+  <si>
+    <t>comColLot</t>
+  </si>
+  <si>
+    <t>comTemplatePosition</t>
+  </si>
+  <si>
+    <t>comColSampling</t>
+  </si>
+  <si>
+    <t>comColRowNum</t>
+  </si>
+  <si>
+    <t>comColData</t>
+  </si>
+  <si>
+    <t>comColMEA</t>
+  </si>
+  <si>
+    <t>comColSheet</t>
+  </si>
+  <si>
+    <t>comTemplateSheet</t>
+  </si>
+  <si>
+    <t>comConfigSheet</t>
+  </si>
+  <si>
+    <t>comPath</t>
+  </si>
+  <si>
+    <t>comMasterPath</t>
+  </si>
+  <si>
+    <t>wipColQty</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>for determine column Qty in wip excel</t>
+  </si>
+  <si>
+    <t>S:\EDP\RPA\RPA Phase7\DDS\Industry4.0\Example Rev.03\03.Output</t>
   </si>
 </sst>
 </file>
@@ -713,12 +1202,54 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -734,7 +1265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -753,6 +1284,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1037,7 +1578,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1600,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1067,12 +1608,12 @@
         <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1080,10 +1621,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -1096,16 +1637,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1118,98 +1659,146 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>327</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>328</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1241,18 +1830,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1262,15 +1851,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1284,34 +1873,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B7" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1321,17 +1926,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1342,378 +1947,973 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C5" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B37" s="14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C37" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="B58" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" t="s">
-        <v>108</v>
-      </c>
-      <c r="C20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>123</v>
-      </c>
-      <c r="B30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>153</v>
-      </c>
-      <c r="B33" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>163</v>
-      </c>
-      <c r="B34" t="s">
-        <v>162</v>
-      </c>
-      <c r="C34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>165</v>
-      </c>
-      <c r="B35" t="s">
-        <v>164</v>
-      </c>
-      <c r="C35" t="s">
-        <v>161</v>
+      <c r="C58" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1727,7 +2927,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,42 +2942,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1809,18 +3009,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1852,34 +3052,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1891,13 +3091,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="19" max="19" width="0.5703125" customWidth="1"/>
@@ -1916,39 +3116,39 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>168</v>
+        <v>119</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>